<commit_message>
refactored trade_algo for better code flow
- deleted unused imports in cagr.analytics_live.py

trade_algo.utils.py
- deleted get_EOD_date() to be done in main() directly
- pep8 formatting using black

trade_algo.run.py
- refactored to do O(1) computation directly in main()
</commit_message>
<xml_diff>
--- a/research/1yr-9mnth-back-2002-jan/stock-2023-01-06.xlsx
+++ b/research/1yr-9mnth-back-2002-jan/stock-2023-01-06.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jimmy\cagr-analysis\research\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jimmy\cagr-analysis\research\1yr-9mnth-back-2002-jan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6639E25-6FBA-4AF6-AEDC-8D8FD9DAB27C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45589DF-1759-4713-A054-D4D1CBE039CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25290" yWindow="3255" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38505" yWindow="-1680" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1544,7 +1557,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1556,6 +1572,13 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1590,17 +1613,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1900,10 +1927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M492"/>
+  <dimension ref="A1:P492"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1923,7 +1950,7 @@
     <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1961,7 +1988,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2001,8 +2028,15 @@
       <c r="M2">
         <v>200.8</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2">
+        <v>5404</v>
+      </c>
+      <c r="O2" s="2">
+        <f>(N2-C2)/C2</f>
+        <v>1.9359193763072826</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2042,8 +2076,15 @@
       <c r="M3">
         <v>176.2</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3">
+        <v>2083</v>
+      </c>
+      <c r="O3" s="2">
+        <f t="shared" ref="O3:O14" si="0">(N3-C3)/C3</f>
+        <v>1.5945070685682257</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2083,8 +2124,15 @@
       <c r="M4">
         <v>154.9</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4">
+        <v>801</v>
+      </c>
+      <c r="O4" s="2">
+        <f t="shared" si="0"/>
+        <v>1.2694432639184021</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2124,8 +2172,15 @@
       <c r="M5">
         <v>123.1</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5">
+        <v>40.75</v>
+      </c>
+      <c r="O5" s="2">
+        <f t="shared" si="0"/>
+        <v>0.31239935587761669</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2165,8 +2220,15 @@
       <c r="M6">
         <v>106.6</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6">
+        <v>170</v>
+      </c>
+      <c r="O6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.54475238527941849</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2206,8 +2268,15 @@
       <c r="M7">
         <v>111.8</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7">
+        <v>183</v>
+      </c>
+      <c r="O7" s="2">
+        <f t="shared" si="0"/>
+        <v>1.525879917184265</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2247,8 +2316,15 @@
       <c r="M8">
         <v>105.3</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8">
+        <v>305</v>
+      </c>
+      <c r="O8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.79570209007948201</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2288,8 +2364,15 @@
       <c r="M9">
         <v>100.2</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9">
+        <v>1099</v>
+      </c>
+      <c r="O9" s="2">
+        <f t="shared" si="0"/>
+        <v>0.68959950803290015</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2329,8 +2412,15 @@
       <c r="M10">
         <v>93.7</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N10">
+        <v>128</v>
+      </c>
+      <c r="O10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.58415841584158423</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2370,8 +2460,15 @@
       <c r="M11">
         <v>102.2</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11">
+        <v>316</v>
+      </c>
+      <c r="O11" s="2">
+        <f t="shared" si="0"/>
+        <v>1.6245847176079733</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2411,8 +2508,19 @@
       <c r="M12">
         <v>94.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12">
+        <v>112.6</v>
+      </c>
+      <c r="O12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.20492241840556438</v>
+      </c>
+      <c r="P12" s="3">
+        <f>AVERAGE(O2:O12)</f>
+        <v>1.007442592463883</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2452,8 +2560,9 @@
       <c r="M13">
         <v>83.8</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O13" s="2"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2493,8 +2602,9 @@
       <c r="M14">
         <v>80.2</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O14" s="2"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2535,7 +2645,7 @@
         <v>77.3</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>

</xml_diff>